<commit_message>
feat:creator mode for testing new color
</commit_message>
<xml_diff>
--- a/ExtremeSkinTransData.xlsx
+++ b/ExtremeSkinTransData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460E495E-7C5A-4949-A38B-282601F2A975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD77922-9118-46D5-A7B7-0C96A4B1D672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hat" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>English</t>
   </si>
@@ -114,6 +114,17 @@
   </si>
   <si>
     <t>コテツ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>configAddColor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テスト追加カラー</t>
+    <rPh sb="3" eb="5">
+      <t>ツイカ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -447,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -562,10 +573,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
-  <dimension ref="B1:Q81"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -574,7 +585,7 @@
     <col min="13" max="13" width="56.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -622,6 +633,14 @@
       </c>
       <c r="Q1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="13:13" ht="21" customHeight="1" x14ac:dyDescent="0.4"/>

</xml_diff>